<commit_message>
working on buds model and seed collection
</commit_message>
<xml_diff>
--- a/data/Seeds_count.xlsx
+++ b/data/Seeds_count.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>Species</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>ALNINC01_HF</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
 </sst>
 </file>
@@ -154,12 +157,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -188,7 +197,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -467,18 +476,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -498,7 +508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -512,7 +522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -526,7 +536,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -540,7 +550,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -554,7 +564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -568,7 +578,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -582,7 +592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -590,13 +600,16 @@
         <v>21</v>
       </c>
       <c r="C8" s="2">
-        <v>42895</v>
+        <v>42164</v>
       </c>
       <c r="D8">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -604,13 +617,13 @@
         <v>22</v>
       </c>
       <c r="C9" s="2">
-        <v>42896</v>
+        <v>42165</v>
       </c>
       <c r="D9">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -624,7 +637,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -638,7 +651,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -652,7 +665,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -666,7 +679,7 @@
         <v>42278</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -677,7 +690,7 @@
         <v>41911</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -688,7 +701,7 @@
         <v>41920</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -733,6 +746,14 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>